<commit_message>
WORK FROM MIUA 2018 DONE
</commit_message>
<xml_diff>
--- a/macros123singles.xlsx
+++ b/macros123singles.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jsolisl\Documents\PhD\SW\macrosight\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsolisl/Documents/PhD/SW/macrosight/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24CF940E-17B7-8842-B6BE-7C5331C8BCEB}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23235" windowHeight="9825"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="17980" windowHeight="10680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -110,7 +111,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1102,27 +1103,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1151,7 +1152,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
@@ -1162,7 +1163,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="6">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E2" s="6">
         <f>'[1]clump-related'!F2-1</f>
@@ -1177,14 +1178,14 @@
       </c>
       <c r="H2" s="6">
         <f>E2-D2</f>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I2" s="8">
         <f>G2-F2</f>
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>10</v>
       </c>
@@ -1206,7 +1207,7 @@
         <v>48</v>
       </c>
       <c r="G3" s="12">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="H3" s="11">
         <f t="shared" ref="H3:H38" si="0">E3-D3</f>
@@ -1214,10 +1215,10 @@
       </c>
       <c r="I3" s="13">
         <f t="shared" ref="I3:I38" si="1">G3-F3</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>11</v>
       </c>
@@ -1239,7 +1240,7 @@
         <v>52</v>
       </c>
       <c r="G4" s="12">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H4" s="11">
         <f t="shared" si="0"/>
@@ -1247,10 +1248,10 @@
       </c>
       <c r="I4" s="13">
         <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>12</v>
       </c>
@@ -1272,7 +1273,7 @@
         <v>52</v>
       </c>
       <c r="G5" s="12">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H5" s="11">
         <f t="shared" si="0"/>
@@ -1280,10 +1281,10 @@
       </c>
       <c r="I5" s="13">
         <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>13</v>
       </c>
@@ -1294,7 +1295,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="11">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="E6" s="11">
         <f>'[1]clump-related'!F6-1</f>
@@ -1305,18 +1306,18 @@
         <v>157</v>
       </c>
       <c r="G6" s="12">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="H6" s="11">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="I6" s="13">
         <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>14</v>
       </c>
@@ -1327,7 +1328,7 @@
         <v>6</v>
       </c>
       <c r="D7" s="11">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="E7" s="11">
         <f>'[1]clump-related'!F7-1</f>
@@ -1342,14 +1343,14 @@
       </c>
       <c r="H7" s="11">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="I7" s="13">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>15</v>
       </c>
@@ -1382,7 +1383,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>16</v>
       </c>
@@ -1415,7 +1416,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
         <v>17</v>
       </c>
@@ -1426,7 +1427,7 @@
         <v>7</v>
       </c>
       <c r="D10" s="11">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E10" s="11">
         <f>'[1]clump-related'!F10-1</f>
@@ -1437,18 +1438,18 @@
         <v>28</v>
       </c>
       <c r="G10" s="12">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H10" s="11">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I10" s="13">
         <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
         <v>18</v>
       </c>
@@ -1459,7 +1460,7 @@
         <v>8</v>
       </c>
       <c r="D11" s="11">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E11" s="11">
         <f>'[1]clump-related'!F11-1</f>
@@ -1470,18 +1471,18 @@
         <v>28</v>
       </c>
       <c r="G11" s="12">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H11" s="11">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I11" s="13">
         <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
         <v>19</v>
       </c>
@@ -1492,7 +1493,7 @@
         <v>7</v>
       </c>
       <c r="D12" s="11">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E12" s="11">
         <f>'[1]clump-related'!F12-1</f>
@@ -1503,18 +1504,18 @@
         <v>49</v>
       </c>
       <c r="G12" s="12">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H12" s="11">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="I12" s="13">
         <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>20</v>
       </c>
@@ -1525,7 +1526,7 @@
         <v>8</v>
       </c>
       <c r="D13" s="11">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E13" s="11">
         <f>'[1]clump-related'!F13-1</f>
@@ -1536,18 +1537,18 @@
         <v>49</v>
       </c>
       <c r="G13" s="12">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H13" s="11">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="I13" s="13">
         <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
         <v>21</v>
       </c>
@@ -1569,7 +1570,7 @@
         <v>56</v>
       </c>
       <c r="G14" s="12">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="H14" s="11">
         <f t="shared" si="0"/>
@@ -1577,10 +1578,10 @@
       </c>
       <c r="I14" s="13">
         <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
         <v>22</v>
       </c>
@@ -1591,7 +1592,7 @@
         <v>2</v>
       </c>
       <c r="D15" s="11">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="E15" s="11">
         <f>'[1]clump-related'!F15-1</f>
@@ -1602,18 +1603,18 @@
         <v>311</v>
       </c>
       <c r="G15" s="12">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="H15" s="11">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I15" s="13">
         <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
         <v>23</v>
       </c>
@@ -1624,7 +1625,7 @@
         <v>19</v>
       </c>
       <c r="D16" s="11">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="E16" s="11">
         <f>'[1]clump-related'!F16-1</f>
@@ -1635,18 +1636,18 @@
         <v>311</v>
       </c>
       <c r="G16" s="12">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="H16" s="11">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I16" s="13">
         <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
         <v>24</v>
       </c>
@@ -1679,7 +1680,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>25</v>
       </c>
@@ -1712,7 +1713,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="str">
         <f>'[1]clump-related'!A19</f>
         <v>macros3-1</v>
@@ -1726,7 +1727,7 @@
         <v>1</v>
       </c>
       <c r="D19" s="6">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="E19" s="6">
         <f>'[1]clump-related'!F19-1</f>
@@ -1741,14 +1742,14 @@
       </c>
       <c r="H19" s="6">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="I19" s="8">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="str">
         <f>'[1]clump-related'!A20</f>
         <v>macros3-2</v>
@@ -1784,7 +1785,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="str">
         <f>'[1]clump-related'!A21</f>
         <v>macros3-3</v>
@@ -1798,7 +1799,7 @@
         <v>2</v>
       </c>
       <c r="D21" s="11">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="E21" s="11">
         <f>'[1]clump-related'!F21-1</f>
@@ -1809,18 +1810,18 @@
         <v>238</v>
       </c>
       <c r="G21" s="12">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="H21" s="11">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="I21" s="13">
         <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="str">
         <f>'[1]clump-related'!A22</f>
         <v>macros3-4</v>
@@ -1834,7 +1835,7 @@
         <v>3</v>
       </c>
       <c r="D22" s="11">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="E22" s="11">
         <f>'[1]clump-related'!F22-1</f>
@@ -1845,18 +1846,18 @@
         <v>238</v>
       </c>
       <c r="G22" s="12">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="H22" s="11">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="I22" s="13">
         <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="str">
         <f>'[1]clump-related'!A23</f>
         <v>macros3-5</v>
@@ -1892,7 +1893,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="str">
         <f>'[1]clump-related'!A24</f>
         <v>macros3-6</v>
@@ -1917,7 +1918,7 @@
         <v>379</v>
       </c>
       <c r="G24" s="12">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="H24" s="11">
         <f t="shared" si="0"/>
@@ -1925,10 +1926,10 @@
       </c>
       <c r="I24" s="13">
         <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="str">
         <f>'[1]clump-related'!A25</f>
         <v>macros3-7</v>
@@ -1953,7 +1954,7 @@
         <v>39</v>
       </c>
       <c r="G25" s="12">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H25" s="11">
         <f t="shared" si="0"/>
@@ -1961,10 +1962,10 @@
       </c>
       <c r="I25" s="13">
         <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="str">
         <f>'[1]clump-related'!A26</f>
         <v>macros3-8</v>
@@ -1989,7 +1990,7 @@
         <v>39</v>
       </c>
       <c r="G26" s="12">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H26" s="11">
         <f t="shared" si="0"/>
@@ -1997,10 +1998,10 @@
       </c>
       <c r="I26" s="13">
         <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="str">
         <f>'[1]clump-related'!A27</f>
         <v>macros3-9</v>
@@ -2014,7 +2015,7 @@
         <v>6</v>
       </c>
       <c r="D27" s="11">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E27" s="11">
         <f>'[1]clump-related'!F27-1</f>
@@ -2025,18 +2026,18 @@
         <v>67</v>
       </c>
       <c r="G27" s="12">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H27" s="11">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I27" s="13">
         <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="str">
         <f>'[1]clump-related'!A28</f>
         <v>macros3-10</v>
@@ -2050,7 +2051,7 @@
         <v>9</v>
       </c>
       <c r="D28" s="11">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E28" s="11">
         <f>'[1]clump-related'!F28-1</f>
@@ -2061,18 +2062,18 @@
         <v>67</v>
       </c>
       <c r="G28" s="12">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H28" s="11">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I28" s="13">
         <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="str">
         <f>'[1]clump-related'!A29</f>
         <v>macros3-11</v>
@@ -2086,7 +2087,7 @@
         <v>5</v>
       </c>
       <c r="D29" s="11">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E29" s="11">
         <f>'[1]clump-related'!F29-1</f>
@@ -2097,18 +2098,18 @@
         <v>95</v>
       </c>
       <c r="G29" s="12">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H29" s="11">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I29" s="13">
         <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="str">
         <f>'[1]clump-related'!A30</f>
         <v>macros3-12</v>
@@ -2122,7 +2123,7 @@
         <v>17</v>
       </c>
       <c r="D30" s="11">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E30" s="11">
         <f>'[1]clump-related'!F30-1</f>
@@ -2137,14 +2138,14 @@
       </c>
       <c r="H30" s="11">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I30" s="13">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="str">
         <f>'[1]clump-related'!A31</f>
         <v>macros3-13</v>
@@ -2158,7 +2159,7 @@
         <v>8</v>
       </c>
       <c r="D31" s="11">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="E31" s="11">
         <f>'[1]clump-related'!F31-1</f>
@@ -2173,14 +2174,14 @@
       </c>
       <c r="H31" s="11">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I31" s="13">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="str">
         <f>'[1]clump-related'!A32</f>
         <v>macros3-14</v>
@@ -2194,7 +2195,7 @@
         <v>19</v>
       </c>
       <c r="D32" s="11">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="E32" s="11">
         <f>'[1]clump-related'!F32-1</f>
@@ -2209,14 +2210,14 @@
       </c>
       <c r="H32" s="11">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I32" s="13">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="str">
         <f>'[1]clump-related'!A33</f>
         <v>macros3-15</v>
@@ -2241,7 +2242,7 @@
         <v>132</v>
       </c>
       <c r="G33" s="12">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H33" s="11">
         <f t="shared" si="0"/>
@@ -2249,10 +2250,10 @@
       </c>
       <c r="I33" s="13">
         <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="str">
         <f>'[1]clump-related'!A34</f>
         <v>macros3-16</v>
@@ -2288,7 +2289,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="str">
         <f>'[1]clump-related'!A35</f>
         <v>macros3-17</v>
@@ -2313,7 +2314,7 @@
         <v>234</v>
       </c>
       <c r="G35" s="12">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="H35" s="11">
         <f t="shared" si="0"/>
@@ -2321,10 +2322,10 @@
       </c>
       <c r="I35" s="13">
         <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="str">
         <f>'[1]clump-related'!A36</f>
         <v>macros3-18</v>
@@ -2349,7 +2350,7 @@
         <v>234</v>
       </c>
       <c r="G36" s="12">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="H36" s="11">
         <f t="shared" si="0"/>
@@ -2357,10 +2358,10 @@
       </c>
       <c r="I36" s="13">
         <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="str">
         <f>'[1]clump-related'!A37</f>
         <v>macros3-19</v>
@@ -2385,7 +2386,7 @@
         <v>46</v>
       </c>
       <c r="G37" s="12">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="H37" s="11">
         <f t="shared" si="0"/>
@@ -2393,10 +2394,10 @@
       </c>
       <c r="I37" s="13">
         <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="str">
         <f>'[1]clump-related'!A38</f>
         <v>macros3-20</v>
@@ -2410,7 +2411,7 @@
         <v>22</v>
       </c>
       <c r="D38" s="16">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="E38" s="16">
         <f>'[1]clump-related'!F38-1</f>
@@ -2421,15 +2422,15 @@
         <v>403</v>
       </c>
       <c r="G38" s="17">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="H38" s="16">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I38" s="18">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Experiments for MACROS 1 ready
</commit_message>
<xml_diff>
--- a/macros123singles.xlsx
+++ b/macros123singles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsolisl/Documents/PhD/SW/macrosight/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jsolisl\Documents\PhD\SW\macrosight\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24CF940E-17B7-8842-B6BE-7C5331C8BCEB}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{59F37AF2-4D1F-4C0F-B259-05E13AB46BA3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="17980" windowHeight="10680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="17985" windowHeight="10680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <externalReferences>
     <externalReference r:id="rId2"/>
   </externalReferences>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>whichdataset</t>
   </si>
@@ -106,6 +106,51 @@
   </si>
   <si>
     <t>MACROS2-17</t>
+  </si>
+  <si>
+    <t>macros1-3</t>
+  </si>
+  <si>
+    <t>macros1-4</t>
+  </si>
+  <si>
+    <t>macros1-15</t>
+  </si>
+  <si>
+    <t>macros1-16</t>
+  </si>
+  <si>
+    <t>macros1-19</t>
+  </si>
+  <si>
+    <t>macros1-20</t>
+  </si>
+  <si>
+    <t>macros1-26</t>
+  </si>
+  <si>
+    <t>macros1-27</t>
+  </si>
+  <si>
+    <t>macros1-28</t>
+  </si>
+  <si>
+    <t>macros1-29</t>
+  </si>
+  <si>
+    <t>macros1-30</t>
+  </si>
+  <si>
+    <t>macros1-31</t>
+  </si>
+  <si>
+    <t>macros1-40</t>
+  </si>
+  <si>
+    <t>macros1-41</t>
+  </si>
+  <si>
+    <t>macros1-42</t>
   </si>
 </sst>
 </file>
@@ -121,7 +166,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -146,8 +191,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -272,11 +323,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -296,6 +427,21 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -800,8 +946,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1104,26 +1250,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39:I53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1152,7 +1298,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
@@ -1185,7 +1331,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>10</v>
       </c>
@@ -1210,15 +1356,15 @@
         <v>59</v>
       </c>
       <c r="H3" s="11">
-        <f t="shared" ref="H3:H38" si="0">E3-D3</f>
+        <f t="shared" ref="H3:H53" si="0">E3-D3</f>
         <v>8</v>
       </c>
       <c r="I3" s="13">
-        <f t="shared" ref="I3:I38" si="1">G3-F3</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <f t="shared" ref="I3:I53" si="1">G3-F3</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>11</v>
       </c>
@@ -1251,7 +1397,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>12</v>
       </c>
@@ -1284,7 +1430,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>13</v>
       </c>
@@ -1317,7 +1463,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>14</v>
       </c>
@@ -1350,7 +1496,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>15</v>
       </c>
@@ -1383,7 +1529,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>16</v>
       </c>
@@ -1416,7 +1562,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>17</v>
       </c>
@@ -1449,7 +1595,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>18</v>
       </c>
@@ -1482,7 +1628,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>19</v>
       </c>
@@ -1515,7 +1661,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>20</v>
       </c>
@@ -1548,7 +1694,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>21</v>
       </c>
@@ -1581,7 +1727,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>22</v>
       </c>
@@ -1614,7 +1760,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>23</v>
       </c>
@@ -1647,7 +1793,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>24</v>
       </c>
@@ -1680,7 +1826,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14" t="s">
         <v>25</v>
       </c>
@@ -1713,7 +1859,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="str">
         <f>'[1]clump-related'!A19</f>
         <v>macros3-1</v>
@@ -1749,7 +1895,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="str">
         <f>'[1]clump-related'!A20</f>
         <v>macros3-2</v>
@@ -1785,7 +1931,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="str">
         <f>'[1]clump-related'!A21</f>
         <v>macros3-3</v>
@@ -1821,7 +1967,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="str">
         <f>'[1]clump-related'!A22</f>
         <v>macros3-4</v>
@@ -1857,7 +2003,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="str">
         <f>'[1]clump-related'!A23</f>
         <v>macros3-5</v>
@@ -1893,7 +2039,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="str">
         <f>'[1]clump-related'!A24</f>
         <v>macros3-6</v>
@@ -1929,7 +2075,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="str">
         <f>'[1]clump-related'!A25</f>
         <v>macros3-7</v>
@@ -1965,7 +2111,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="str">
         <f>'[1]clump-related'!A26</f>
         <v>macros3-8</v>
@@ -2001,7 +2147,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="str">
         <f>'[1]clump-related'!A27</f>
         <v>macros3-9</v>
@@ -2037,7 +2183,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="str">
         <f>'[1]clump-related'!A28</f>
         <v>macros3-10</v>
@@ -2073,7 +2219,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="str">
         <f>'[1]clump-related'!A29</f>
         <v>macros3-11</v>
@@ -2109,7 +2255,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="str">
         <f>'[1]clump-related'!A30</f>
         <v>macros3-12</v>
@@ -2145,7 +2291,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="str">
         <f>'[1]clump-related'!A31</f>
         <v>macros3-13</v>
@@ -2181,7 +2327,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="str">
         <f>'[1]clump-related'!A32</f>
         <v>macros3-14</v>
@@ -2217,7 +2363,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="str">
         <f>'[1]clump-related'!A33</f>
         <v>macros3-15</v>
@@ -2253,7 +2399,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="str">
         <f>'[1]clump-related'!A34</f>
         <v>macros3-16</v>
@@ -2289,7 +2435,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="str">
         <f>'[1]clump-related'!A35</f>
         <v>macros3-17</v>
@@ -2325,7 +2471,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="str">
         <f>'[1]clump-related'!A36</f>
         <v>macros3-18</v>
@@ -2361,7 +2507,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="str">
         <f>'[1]clump-related'!A37</f>
         <v>macros3-19</v>
@@ -2397,40 +2543,505 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="14" t="str">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="9" t="str">
         <f>'[1]clump-related'!A38</f>
         <v>macros3-20</v>
       </c>
-      <c r="B38" s="15">
+      <c r="B38" s="10">
         <f>'[1]clump-related'!B38</f>
         <v>22001</v>
       </c>
-      <c r="C38" s="15">
+      <c r="C38" s="10">
         <f>'[1]clump-related'!C38</f>
         <v>22</v>
       </c>
-      <c r="D38" s="16">
+      <c r="D38" s="11">
         <v>388</v>
       </c>
-      <c r="E38" s="16">
+      <c r="E38" s="11">
         <f>'[1]clump-related'!F38-1</f>
         <v>399</v>
       </c>
-      <c r="F38" s="17">
+      <c r="F38" s="12">
         <f>'[1]clump-related'!G38+1</f>
         <v>403</v>
       </c>
-      <c r="G38" s="17">
+      <c r="G38" s="12">
         <v>414</v>
       </c>
-      <c r="H38" s="16">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="I38" s="18">
-        <f t="shared" si="1"/>
-        <v>11</v>
+      <c r="H38" s="11">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="I38" s="13">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B39" s="21">
+        <v>8002</v>
+      </c>
+      <c r="C39" s="21">
+        <v>2</v>
+      </c>
+      <c r="D39" s="22">
+        <v>407</v>
+      </c>
+      <c r="E39" s="22">
+        <v>417</v>
+      </c>
+      <c r="F39" s="32">
+        <v>418</v>
+      </c>
+      <c r="G39" s="32">
+        <v>427</v>
+      </c>
+      <c r="H39" s="22">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I39" s="23">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B40" s="19">
+        <v>8002</v>
+      </c>
+      <c r="C40" s="19">
+        <v>8</v>
+      </c>
+      <c r="D40" s="11">
+        <v>407</v>
+      </c>
+      <c r="E40" s="11">
+        <v>417</v>
+      </c>
+      <c r="F40" s="12">
+        <v>418</v>
+      </c>
+      <c r="G40" s="12">
+        <v>427</v>
+      </c>
+      <c r="H40" s="11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I40" s="25">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B41" s="19">
+        <v>20001</v>
+      </c>
+      <c r="C41" s="10">
+        <v>1</v>
+      </c>
+      <c r="D41" s="11">
+        <v>103</v>
+      </c>
+      <c r="E41" s="11">
+        <v>113</v>
+      </c>
+      <c r="F41" s="12">
+        <v>122</v>
+      </c>
+      <c r="G41" s="12">
+        <v>131</v>
+      </c>
+      <c r="H41" s="11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I41" s="25">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B42" s="19">
+        <v>20001</v>
+      </c>
+      <c r="C42" s="10">
+        <v>20</v>
+      </c>
+      <c r="D42" s="11">
+        <v>103</v>
+      </c>
+      <c r="E42" s="11">
+        <v>113</v>
+      </c>
+      <c r="F42" s="12">
+        <v>122</v>
+      </c>
+      <c r="G42" s="12">
+        <v>131</v>
+      </c>
+      <c r="H42" s="11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I42" s="25">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B43" s="19">
+        <v>20005</v>
+      </c>
+      <c r="C43" s="10">
+        <v>5</v>
+      </c>
+      <c r="D43" s="11">
+        <v>89</v>
+      </c>
+      <c r="E43" s="11">
+        <v>99</v>
+      </c>
+      <c r="F43" s="12">
+        <v>100</v>
+      </c>
+      <c r="G43" s="12">
+        <v>109</v>
+      </c>
+      <c r="H43" s="11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I43" s="25">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B44" s="19">
+        <v>20005</v>
+      </c>
+      <c r="C44" s="10">
+        <v>20</v>
+      </c>
+      <c r="D44" s="11">
+        <v>89</v>
+      </c>
+      <c r="E44" s="11">
+        <v>99</v>
+      </c>
+      <c r="F44" s="12">
+        <v>100</v>
+      </c>
+      <c r="G44" s="12">
+        <v>109</v>
+      </c>
+      <c r="H44" s="11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I44" s="25">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B45" s="19">
+        <v>50002</v>
+      </c>
+      <c r="C45" s="10">
+        <v>2</v>
+      </c>
+      <c r="D45" s="11">
+        <v>166</v>
+      </c>
+      <c r="E45" s="11">
+        <v>176</v>
+      </c>
+      <c r="F45" s="12">
+        <v>179</v>
+      </c>
+      <c r="G45" s="12">
+        <v>188</v>
+      </c>
+      <c r="H45" s="11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I45" s="25">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B46" s="19">
+        <v>50002</v>
+      </c>
+      <c r="C46" s="10">
+        <v>50</v>
+      </c>
+      <c r="D46" s="11">
+        <v>166</v>
+      </c>
+      <c r="E46" s="11">
+        <v>176</v>
+      </c>
+      <c r="F46" s="12">
+        <v>179</v>
+      </c>
+      <c r="G46" s="12">
+        <v>183</v>
+      </c>
+      <c r="H46" s="11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I46" s="25">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B47" s="19">
+        <v>60002</v>
+      </c>
+      <c r="C47" s="10">
+        <v>2</v>
+      </c>
+      <c r="D47" s="11">
+        <v>377</v>
+      </c>
+      <c r="E47" s="11">
+        <v>387</v>
+      </c>
+      <c r="F47" s="12">
+        <v>388</v>
+      </c>
+      <c r="G47" s="12">
+        <v>397</v>
+      </c>
+      <c r="H47" s="11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I47" s="25">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B48" s="19">
+        <v>60002</v>
+      </c>
+      <c r="C48" s="10">
+        <v>60</v>
+      </c>
+      <c r="D48" s="11">
+        <v>377</v>
+      </c>
+      <c r="E48" s="11">
+        <v>387</v>
+      </c>
+      <c r="F48" s="12">
+        <v>388</v>
+      </c>
+      <c r="G48" s="12">
+        <v>397</v>
+      </c>
+      <c r="H48" s="11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I48" s="25">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B49" s="19">
+        <v>60008</v>
+      </c>
+      <c r="C49" s="10">
+        <v>8</v>
+      </c>
+      <c r="D49" s="11">
+        <v>478</v>
+      </c>
+      <c r="E49" s="11">
+        <v>488</v>
+      </c>
+      <c r="F49" s="12">
+        <v>494</v>
+      </c>
+      <c r="G49" s="12">
+        <v>503</v>
+      </c>
+      <c r="H49" s="11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I49" s="25">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B50" s="19">
+        <v>60008</v>
+      </c>
+      <c r="C50" s="10">
+        <v>60</v>
+      </c>
+      <c r="D50" s="11">
+        <v>478</v>
+      </c>
+      <c r="E50" s="11">
+        <v>488</v>
+      </c>
+      <c r="F50" s="12">
+        <v>494</v>
+      </c>
+      <c r="G50" s="12">
+        <v>503</v>
+      </c>
+      <c r="H50" s="11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I50" s="25">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="B51" s="19">
+        <v>77070</v>
+      </c>
+      <c r="C51" s="10">
+        <v>70</v>
+      </c>
+      <c r="D51" s="11">
+        <v>409</v>
+      </c>
+      <c r="E51" s="11">
+        <v>419</v>
+      </c>
+      <c r="F51" s="12">
+        <v>428</v>
+      </c>
+      <c r="G51" s="12">
+        <v>437</v>
+      </c>
+      <c r="H51" s="11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I51" s="25">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B52" s="19">
+        <v>77070</v>
+      </c>
+      <c r="C52" s="10">
+        <v>70</v>
+      </c>
+      <c r="D52" s="11">
+        <v>409</v>
+      </c>
+      <c r="E52" s="11">
+        <v>419</v>
+      </c>
+      <c r="F52" s="12">
+        <v>428</v>
+      </c>
+      <c r="G52" s="12">
+        <v>437</v>
+      </c>
+      <c r="H52" s="11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I52" s="25">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="B53" s="28">
+        <v>84083</v>
+      </c>
+      <c r="C53" s="29">
+        <v>83</v>
+      </c>
+      <c r="D53" s="30">
+        <v>416</v>
+      </c>
+      <c r="E53" s="30">
+        <v>426</v>
+      </c>
+      <c r="F53" s="33">
+        <v>428</v>
+      </c>
+      <c r="G53" s="33">
+        <v>437</v>
+      </c>
+      <c r="H53" s="30">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I53" s="31">
+        <f t="shared" si="1"/>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>